<commit_message>
Update of dutch translations
</commit_message>
<xml_diff>
--- a/localisation/App_Localization.xlsx
+++ b/localisation/App_Localization.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="11760" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="416">
   <si>
     <t>Meeting App</t>
   </si>
@@ -654,132 +654,12 @@
     <t>Gehgeschwindigkeit</t>
   </si>
   <si>
-    <t>komende bijeenkomsten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nieuwe afspraak </t>
-  </si>
-  <si>
-    <t>contacten</t>
-  </si>
-  <si>
-    <t>uitloggen</t>
-  </si>
-  <si>
-    <t>opzicht</t>
-  </si>
-  <si>
-    <t>datum</t>
-  </si>
-  <si>
-    <t>tijdstip</t>
-  </si>
-  <si>
-    <t>plaats</t>
-  </si>
-  <si>
-    <t>contactpersonen toevoegen</t>
-  </si>
-  <si>
-    <t>stuur afspraak</t>
-  </si>
-  <si>
-    <t>geselecteerde contactpersonen</t>
-  </si>
-  <si>
-    <t>Toegevoegd contacten</t>
-  </si>
-  <si>
-    <t>wachtwoord</t>
-  </si>
-  <si>
-    <t>inschrijven</t>
-  </si>
-  <si>
-    <t>groepen</t>
-  </si>
-  <si>
-    <t>update</t>
-  </si>
-  <si>
-    <t>groep maken</t>
-  </si>
-  <si>
-    <t>beschrijving</t>
-  </si>
-  <si>
     <t>Maakt verbinding met server</t>
   </si>
   <si>
-    <t>login succesvol</t>
-  </si>
-  <si>
-    <t>je profiel</t>
-  </si>
-  <si>
-    <t>persoonlijk</t>
-  </si>
-  <si>
-    <t>voornaam</t>
-  </si>
-  <si>
-    <t>tweede naam</t>
-  </si>
-  <si>
-    <t>achternaam</t>
-  </si>
-  <si>
-    <t>geslacht</t>
-  </si>
-  <si>
-    <t>mannelijk</t>
-  </si>
-  <si>
-    <t>vrouw</t>
-  </si>
-  <si>
-    <t>verjaardag</t>
-  </si>
-  <si>
     <t>Contact informatie</t>
   </si>
   <si>
-    <t>gebruikersnaam</t>
-  </si>
-  <si>
-    <t>telefoonnummer</t>
-  </si>
-  <si>
-    <t>Gsm- nummer</t>
-  </si>
-  <si>
-    <t>residentie</t>
-  </si>
-  <si>
-    <t>straat</t>
-  </si>
-  <si>
-    <t>huisnummer</t>
-  </si>
-  <si>
-    <t>postcode</t>
-  </si>
-  <si>
-    <t>staat</t>
-  </si>
-  <si>
-    <t>land</t>
-  </si>
-  <si>
-    <t>postadres</t>
-  </si>
-  <si>
-    <t>nadere inlichtingen</t>
-  </si>
-  <si>
-    <t>nationaliteit</t>
-  </si>
-  <si>
     <t>Brits</t>
   </si>
   <si>
@@ -798,144 +678,12 @@
     <t>Spaans</t>
   </si>
   <si>
-    <t>taal</t>
-  </si>
-  <si>
-    <t>burgerlijke staat</t>
-  </si>
-  <si>
-    <t>getrouwd</t>
-  </si>
-  <si>
-    <t>single</t>
-  </si>
-  <si>
-    <t>weduwe</t>
-  </si>
-  <si>
-    <t>onderwijs</t>
-  </si>
-  <si>
-    <t>leerplichtige</t>
-  </si>
-  <si>
-    <t>middelbare scholen</t>
-  </si>
-  <si>
-    <t>gevorderd niveau</t>
-  </si>
-  <si>
-    <t>tertiair</t>
-  </si>
-  <si>
-    <t>doctor</t>
-  </si>
-  <si>
-    <t>arbeidsverhouding</t>
-  </si>
-  <si>
-    <t>werknemers</t>
-  </si>
-  <si>
-    <t>gepensioneerd</t>
-  </si>
-  <si>
-    <t>werkloos</t>
-  </si>
-  <si>
-    <t>beroep</t>
-  </si>
-  <si>
-    <t>leraar</t>
-  </si>
-  <si>
-    <t>ingenieur</t>
-  </si>
-  <si>
-    <t>advocaat</t>
-  </si>
-  <si>
-    <t>ziektekostenverzekering</t>
-  </si>
-  <si>
-    <t>part verzekering</t>
-  </si>
-  <si>
-    <t>volledig verzekerd</t>
-  </si>
-  <si>
-    <t>rolstoel</t>
-  </si>
-  <si>
-    <t>rollator</t>
-  </si>
-  <si>
-    <t>kruk</t>
-  </si>
-  <si>
-    <t>gezond</t>
-  </si>
-  <si>
     <t>Algemene informatie</t>
   </si>
   <si>
-    <t>verwantschap</t>
-  </si>
-  <si>
-    <t>verpleegster</t>
-  </si>
-  <si>
-    <t>verzorger</t>
-  </si>
-  <si>
-    <t>moeder</t>
-  </si>
-  <si>
-    <t>vader</t>
-  </si>
-  <si>
-    <t>verwant</t>
-  </si>
-  <si>
-    <t>anders</t>
-  </si>
-  <si>
-    <t>Machtigingen bewerken</t>
-  </si>
-  <si>
-    <t>gezondheid</t>
-  </si>
-  <si>
-    <t>temperatuur</t>
-  </si>
-  <si>
-    <t>pols</t>
-  </si>
-  <si>
-    <t>Beats per minuut (bpm)</t>
-  </si>
-  <si>
-    <t>loopsnelheid</t>
-  </si>
-  <si>
     <t>Stappen per minuut (spm)</t>
   </si>
   <si>
-    <t>lichaamshouding</t>
-  </si>
-  <si>
-    <t>sluimerend</t>
-  </si>
-  <si>
-    <t>besparen</t>
-  </si>
-  <si>
-    <t>instellingen</t>
-  </si>
-  <si>
-    <t>server instellingen</t>
-  </si>
-  <si>
     <t>rendez-vous prévus</t>
   </si>
   <si>
@@ -1228,6 +976,294 @@
   </si>
   <si>
     <t>Paramètres du serveur</t>
+  </si>
+  <si>
+    <t>Group description</t>
+  </si>
+  <si>
+    <t>Size of Group</t>
+  </si>
+  <si>
+    <t>Les membres du groupe</t>
+  </si>
+  <si>
+    <t>Gruppenmitglieder</t>
+  </si>
+  <si>
+    <t>Leave this group</t>
+  </si>
+  <si>
+    <t>Gruppe verlassen</t>
+  </si>
+  <si>
+    <t>groupe de congé</t>
+  </si>
+  <si>
+    <t>Description du groupe</t>
+  </si>
+  <si>
+    <t>Beschreibung der Gruppe</t>
+  </si>
+  <si>
+    <t>stuur uitnodiging</t>
+  </si>
+  <si>
+    <t>Uit te nodigen contacten</t>
+  </si>
+  <si>
+    <t>Aanmelden</t>
+  </si>
+  <si>
+    <t>Actualiseren</t>
+  </si>
+  <si>
+    <t>Komende bijeenkomsten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maak een nieuwe afspraak </t>
+  </si>
+  <si>
+    <t>Contacten</t>
+  </si>
+  <si>
+    <t>Uitloggen</t>
+  </si>
+  <si>
+    <t>Onderwerp</t>
+  </si>
+  <si>
+    <t>Groepen</t>
+  </si>
+  <si>
+    <t>Tijdstip</t>
+  </si>
+  <si>
+    <t>Plaats</t>
+  </si>
+  <si>
+    <t>Contactpersonen toevoegen</t>
+  </si>
+  <si>
+    <t>Geselecteerde contactpersonen</t>
+  </si>
+  <si>
+    <t>Wachtwoord</t>
+  </si>
+  <si>
+    <t>Groep maken</t>
+  </si>
+  <si>
+    <t>Beschrijving</t>
+  </si>
+  <si>
+    <t>Groepsbeschrijving</t>
+  </si>
+  <si>
+    <t>Grootte van de groep</t>
+  </si>
+  <si>
+    <t>Verlaat groep</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Login succe vol</t>
+  </si>
+  <si>
+    <t>Jouw profiel</t>
+  </si>
+  <si>
+    <t>Persoonlijk</t>
+  </si>
+  <si>
+    <t>Voornaam</t>
+  </si>
+  <si>
+    <t>Tweede naam</t>
+  </si>
+  <si>
+    <t>Achternaam</t>
+  </si>
+  <si>
+    <t>Voorkeursnaam</t>
+  </si>
+  <si>
+    <t>Geslacht</t>
+  </si>
+  <si>
+    <t>Mannelijk</t>
+  </si>
+  <si>
+    <t>Vrouwelijk</t>
+  </si>
+  <si>
+    <t>Verjaardag</t>
+  </si>
+  <si>
+    <t>Gebruikersnaam</t>
+  </si>
+  <si>
+    <t>Telefoonnummer</t>
+  </si>
+  <si>
+    <t>Mobiel nummer</t>
+  </si>
+  <si>
+    <t>Woonadres</t>
+  </si>
+  <si>
+    <t>Straat</t>
+  </si>
+  <si>
+    <t>Huisnummer</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>Staat</t>
+  </si>
+  <si>
+    <t>Postadres</t>
+  </si>
+  <si>
+    <t>Verdere informatie</t>
+  </si>
+  <si>
+    <t>Nationaliteit</t>
+  </si>
+  <si>
+    <t>Taal</t>
+  </si>
+  <si>
+    <t>Burgerlijke staat</t>
+  </si>
+  <si>
+    <t>Getrouwd</t>
+  </si>
+  <si>
+    <t>Weduwe/Weduwnaar</t>
+  </si>
+  <si>
+    <t>Onderwijsniveau</t>
+  </si>
+  <si>
+    <t>Hoogste opleiding</t>
+  </si>
+  <si>
+    <t>Lager middelbaar</t>
+  </si>
+  <si>
+    <t>Hoger middelbaar</t>
+  </si>
+  <si>
+    <t>Na de middelbare</t>
+  </si>
+  <si>
+    <t>Hoger</t>
+  </si>
+  <si>
+    <t>Masteropleiding</t>
+  </si>
+  <si>
+    <t>Arbeidssituatie</t>
+  </si>
+  <si>
+    <t>Loondienst</t>
+  </si>
+  <si>
+    <t>Gepensioneerd</t>
+  </si>
+  <si>
+    <t>Werkloos</t>
+  </si>
+  <si>
+    <t>Beroep</t>
+  </si>
+  <si>
+    <t>Leraar</t>
+  </si>
+  <si>
+    <t>Advocaat</t>
+  </si>
+  <si>
+    <t>Ziektekostenverzekering</t>
+  </si>
+  <si>
+    <t>Gedeeltelijk</t>
+  </si>
+  <si>
+    <t>Volledig verzekerd</t>
+  </si>
+  <si>
+    <t>Mobiliteit niveau</t>
+  </si>
+  <si>
+    <t>Rolstoel</t>
+  </si>
+  <si>
+    <t>Kruk/Wandelstok</t>
+  </si>
+  <si>
+    <t>Gezond</t>
+  </si>
+  <si>
+    <t>Relatie</t>
+  </si>
+  <si>
+    <t>Verzorger</t>
+  </si>
+  <si>
+    <t>Verpleegster</t>
+  </si>
+  <si>
+    <t>Moeder</t>
+  </si>
+  <si>
+    <t>Vader</t>
+  </si>
+  <si>
+    <t>Verwant</t>
+  </si>
+  <si>
+    <t>Anders</t>
+  </si>
+  <si>
+    <t>Toegangs rechten bewerken</t>
+  </si>
+  <si>
+    <t>Gezondheid</t>
+  </si>
+  <si>
+    <t>Temperatuur</t>
+  </si>
+  <si>
+    <t>Ademhalingsfrequentie</t>
+  </si>
+  <si>
+    <t>Hartslag</t>
+  </si>
+  <si>
+    <t>Aantal slagen per minuut</t>
+  </si>
+  <si>
+    <t>Loopsnelheid</t>
+  </si>
+  <si>
+    <t>Lichaamsbouw</t>
+  </si>
+  <si>
+    <t>Rustend</t>
+  </si>
+  <si>
+    <t>Besparen</t>
+  </si>
+  <si>
+    <t>Instellingen</t>
+  </si>
+  <si>
+    <t>Server instellingen</t>
   </si>
 </sst>
 </file>
@@ -1287,16 +1323,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1598,11 +1639,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B94" sqref="B94"/>
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,23 +1672,23 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>306</v>
+      <c r="B3" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>333</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -1657,11 +1698,11 @@
       <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="C4" t="s">
-        <v>213</v>
+      <c r="B4" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>334</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -1671,11 +1712,11 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>214</v>
+        <v>335</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -1685,11 +1726,11 @@
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>308</v>
+      <c r="B6" s="3" t="s">
+        <v>224</v>
       </c>
       <c r="C6" t="s">
-        <v>215</v>
+        <v>336</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -1699,11 +1740,11 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="C7" t="s">
-        <v>216</v>
+      <c r="B7" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>337</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -1713,11 +1754,11 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>217</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -1727,11 +1768,11 @@
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>329</v>
+      <c r="B9" s="3" t="s">
+        <v>245</v>
       </c>
       <c r="C9" t="s">
-        <v>218</v>
+        <v>339</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
@@ -1741,11 +1782,11 @@
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>330</v>
+      <c r="B10" s="3" t="s">
+        <v>246</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>219</v>
+        <v>340</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
@@ -1755,11 +1796,11 @@
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>331</v>
+      <c r="B11" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="C11" t="s">
-        <v>220</v>
+        <v>341</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -1769,11 +1810,11 @@
       <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="C12" t="s">
-        <v>221</v>
+      <c r="B12" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>329</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
@@ -1783,11 +1824,11 @@
       <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>333</v>
+      <c r="B13" s="3" t="s">
+        <v>249</v>
       </c>
       <c r="C13" t="s">
-        <v>222</v>
+        <v>342</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
@@ -1797,11 +1838,11 @@
       <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="C14" t="s">
-        <v>223</v>
+      <c r="B14" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>330</v>
       </c>
       <c r="D14" t="s">
         <v>29</v>
@@ -1811,11 +1852,11 @@
       <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>334</v>
+      <c r="B15" s="3" t="s">
+        <v>250</v>
       </c>
       <c r="C15" t="s">
-        <v>224</v>
+        <v>343</v>
       </c>
       <c r="D15" t="s">
         <v>31</v>
@@ -1825,34 +1866,34 @@
       <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="C16" t="s">
-        <v>225</v>
+      <c r="B16" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>331</v>
       </c>
       <c r="D16" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>336</v>
+      <c r="B18" s="3" t="s">
+        <v>252</v>
       </c>
       <c r="C18" t="s">
-        <v>226</v>
+        <v>338</v>
       </c>
       <c r="D18" t="s">
         <v>36</v>
@@ -1862,11 +1903,11 @@
       <c r="A19" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="C19" t="s">
-        <v>227</v>
+      <c r="B19" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>332</v>
       </c>
       <c r="D19" t="s">
         <v>38</v>
@@ -1876,11 +1917,11 @@
       <c r="A20" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>310</v>
+      <c r="B20" s="3" t="s">
+        <v>226</v>
       </c>
       <c r="C20" t="s">
-        <v>228</v>
+        <v>344</v>
       </c>
       <c r="D20" t="s">
         <v>40</v>
@@ -1890,11 +1931,11 @@
       <c r="A21" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>308</v>
+      <c r="B21" s="3" t="s">
+        <v>224</v>
       </c>
       <c r="C21" t="s">
-        <v>215</v>
+        <v>336</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
@@ -1904,11 +1945,11 @@
       <c r="A22" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="C22" t="s">
-        <v>216</v>
+      <c r="B22" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>337</v>
       </c>
       <c r="D22" t="s">
         <v>14</v>
@@ -1918,11 +1959,11 @@
       <c r="A23" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>229</v>
+        <v>345</v>
       </c>
       <c r="D23" t="s">
         <v>42</v>
@@ -1930,1298 +1971,1340 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>334</v>
+        <v>320</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>327</v>
       </c>
       <c r="C24" t="s">
-        <v>224</v>
+        <v>346</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>328</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>335</v>
+        <v>321</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>322</v>
       </c>
       <c r="C25" t="s">
-        <v>225</v>
+        <v>347</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>323</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="A26" t="s">
+        <v>324</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C26" t="s">
+        <v>348</v>
+      </c>
+      <c r="D26" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>311</v>
+        <v>30</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>250</v>
       </c>
       <c r="C27" t="s">
-        <v>230</v>
+        <v>349</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="C28" t="s">
-        <v>231</v>
+        <v>32</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>331</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C29" t="s">
-        <v>232</v>
-      </c>
-      <c r="D29" t="s">
-        <v>49</v>
-      </c>
+      <c r="A29" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>340</v>
+        <v>44</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>227</v>
       </c>
       <c r="C30" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="D30" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="C31" t="s">
-        <v>234</v>
+        <v>45</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>350</v>
       </c>
       <c r="D31" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="C32" t="s">
-        <v>235</v>
+        <v>48</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>351</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>343</v>
+        <v>50</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>256</v>
       </c>
       <c r="C33" t="s">
-        <v>236</v>
+        <v>352</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>344</v>
+        <v>52</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>257</v>
       </c>
       <c r="C34" t="s">
-        <v>59</v>
+        <v>353</v>
       </c>
       <c r="D34" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>345</v>
+        <v>54</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>258</v>
       </c>
       <c r="C35" t="s">
-        <v>237</v>
+        <v>354</v>
       </c>
       <c r="D35" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>346</v>
+        <v>56</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>259</v>
       </c>
       <c r="C36" t="s">
-        <v>238</v>
+        <v>355</v>
       </c>
       <c r="D36" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="C37" t="s">
-        <v>239</v>
+        <v>58</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>356</v>
       </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>312</v>
+        <v>60</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>261</v>
       </c>
       <c r="C38" t="s">
-        <v>240</v>
+        <v>357</v>
       </c>
       <c r="D38" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>313</v>
+        <v>62</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>262</v>
       </c>
       <c r="C39" t="s">
-        <v>241</v>
+        <v>358</v>
       </c>
       <c r="D39" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="C40" t="s">
-        <v>242</v>
+        <v>64</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>359</v>
       </c>
       <c r="D40" t="s">
-        <v>206</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="C41" t="s">
-        <v>71</v>
+        <v>360</v>
       </c>
       <c r="D41" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>349</v>
+        <v>68</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>229</v>
       </c>
       <c r="C42" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="D42" t="s">
-        <v>207</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>73</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>350</v>
+        <v>70</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>264</v>
       </c>
       <c r="C43" t="s">
-        <v>244</v>
+        <v>361</v>
       </c>
       <c r="D43" t="s">
-        <v>74</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>75</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>314</v>
+        <v>71</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C44" t="s">
-        <v>245</v>
+        <v>71</v>
       </c>
       <c r="D44" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>77</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>351</v>
+        <v>72</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="C45" t="s">
-        <v>246</v>
+        <v>362</v>
       </c>
       <c r="D45" t="s">
-        <v>78</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>79</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="C46" t="s">
-        <v>247</v>
+        <v>73</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>363</v>
       </c>
       <c r="D46" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>81</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="C47" t="s">
-        <v>248</v>
+        <v>75</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>364</v>
       </c>
       <c r="D47" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>88</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>354</v>
+        <v>77</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>267</v>
       </c>
       <c r="C48" t="s">
-        <v>249</v>
+        <v>365</v>
       </c>
       <c r="D48" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>83</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>315</v>
+        <v>79</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>268</v>
       </c>
       <c r="C49" t="s">
-        <v>219</v>
+        <v>366</v>
       </c>
       <c r="D49" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>84</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>316</v>
+        <v>81</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>269</v>
       </c>
       <c r="C50" t="s">
-        <v>250</v>
+        <v>367</v>
       </c>
       <c r="D50" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>86</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>355</v>
+        <v>88</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>270</v>
       </c>
       <c r="C51" t="s">
-        <v>251</v>
+        <v>368</v>
       </c>
       <c r="D51" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>81</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>248</v>
+        <v>83</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C52" t="s">
+        <v>340</v>
       </c>
       <c r="D52" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>90</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>356</v>
+        <v>84</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>232</v>
       </c>
       <c r="C53" t="s">
-        <v>252</v>
+        <v>85</v>
       </c>
       <c r="D53" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>92</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>357</v>
+        <v>86</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>271</v>
       </c>
       <c r="C54" t="s">
-        <v>253</v>
+        <v>369</v>
       </c>
       <c r="D54" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>94</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="C55" t="s">
-        <v>254</v>
+        <v>81</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>367</v>
       </c>
       <c r="D55" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>3</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="C56" t="s">
-        <v>255</v>
+        <v>90</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>370</v>
       </c>
       <c r="D56" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>2</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>360</v>
+        <v>92</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>273</v>
       </c>
       <c r="C57" t="s">
-        <v>256</v>
+        <v>371</v>
       </c>
       <c r="D57" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>361</v>
+        <v>94</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>274</v>
       </c>
       <c r="C58" t="s">
-        <v>257</v>
+        <v>214</v>
       </c>
       <c r="D58" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>362</v>
+        <v>3</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>275</v>
       </c>
       <c r="C59" t="s">
-        <v>258</v>
+        <v>215</v>
       </c>
       <c r="D59" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>100</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>357</v>
+        <v>2</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>276</v>
       </c>
       <c r="C60" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
       <c r="D60" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>102</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>363</v>
+        <v>5</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>277</v>
       </c>
       <c r="C61" t="s">
-        <v>259</v>
+        <v>217</v>
       </c>
       <c r="D61" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>104</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>364</v>
+        <v>4</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>278</v>
       </c>
       <c r="C62" t="s">
-        <v>260</v>
+        <v>218</v>
       </c>
       <c r="D62" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>106</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>317</v>
+        <v>100</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>273</v>
       </c>
       <c r="C63" t="s">
-        <v>261</v>
+        <v>371</v>
       </c>
       <c r="D63" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>108</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>365</v>
+        <v>102</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>279</v>
       </c>
       <c r="C64" t="s">
-        <v>262</v>
+        <v>219</v>
       </c>
       <c r="D64" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>110</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>366</v>
+        <v>104</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>280</v>
       </c>
       <c r="C65" t="s">
-        <v>263</v>
+        <v>372</v>
       </c>
       <c r="D65" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>112</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>367</v>
+        <v>106</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>233</v>
       </c>
       <c r="C66" t="s">
-        <v>264</v>
+        <v>373</v>
       </c>
       <c r="D66" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>114</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>368</v>
+        <v>108</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>281</v>
       </c>
       <c r="C67" t="s">
-        <v>265</v>
+        <v>374</v>
       </c>
       <c r="D67" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>116</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>318</v>
+        <v>110</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>282</v>
       </c>
       <c r="C68" t="s">
-        <v>266</v>
+        <v>110</v>
       </c>
       <c r="D68" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>119</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="C69" t="s">
-        <v>267</v>
+        <v>112</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>375</v>
       </c>
       <c r="D69" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>120</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="C70" t="s">
-        <v>268</v>
+        <v>114</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>376</v>
       </c>
       <c r="D70" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>122</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="C71" t="s">
-        <v>123</v>
+        <v>116</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>377</v>
       </c>
       <c r="D71" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>124</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="C72" t="s">
-        <v>269</v>
+        <v>119</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>378</v>
       </c>
       <c r="D72" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>126</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="C73" t="s">
-        <v>127</v>
+        <v>120</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>379</v>
       </c>
       <c r="D73" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>128</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="C74" t="s">
-        <v>129</v>
+        <v>122</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>380</v>
       </c>
       <c r="D74" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>130</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>373</v>
-      </c>
-      <c r="C75" t="s">
-        <v>270</v>
+        <v>124</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>381</v>
       </c>
       <c r="D75" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>132</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="C76" t="s">
-        <v>271</v>
+        <v>126</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="D76" t="s">
-        <v>208</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>133</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="C77" t="s">
-        <v>272</v>
+        <v>128</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>382</v>
       </c>
       <c r="D77" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>135</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>375</v>
+        <v>130</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>289</v>
       </c>
       <c r="C78" t="s">
-        <v>273</v>
+        <v>169</v>
       </c>
       <c r="D78" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>136</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="C79" t="s">
-        <v>274</v>
+        <v>132</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>383</v>
       </c>
       <c r="D79" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>139</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C80" t="s">
-        <v>275</v>
+        <v>133</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="D80" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>141</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>377</v>
+        <v>135</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>291</v>
       </c>
       <c r="C81" t="s">
-        <v>276</v>
+        <v>385</v>
       </c>
       <c r="D81" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>143</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>378</v>
+        <v>136</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>292</v>
       </c>
       <c r="C82" t="s">
-        <v>277</v>
+        <v>386</v>
       </c>
       <c r="D82" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>145</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>379</v>
+        <v>139</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="C83" t="s">
-        <v>278</v>
+        <v>387</v>
       </c>
       <c r="D83" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>147</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>322</v>
+        <v>141</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>293</v>
       </c>
       <c r="C84" t="s">
-        <v>279</v>
+        <v>388</v>
       </c>
       <c r="D84" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>149</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>380</v>
+        <v>143</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="C85" t="s">
-        <v>280</v>
+        <v>144</v>
       </c>
       <c r="D85" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>151</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>381</v>
+        <v>145</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="C86" t="s">
-        <v>281</v>
+        <v>389</v>
       </c>
       <c r="D86" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>153</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>382</v>
+        <v>147</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>238</v>
       </c>
       <c r="C87" t="s">
-        <v>154</v>
+        <v>390</v>
       </c>
       <c r="D87" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>155</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="C88" t="s">
-        <v>282</v>
+        <v>149</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>391</v>
       </c>
       <c r="D88" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>157</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>384</v>
+        <v>151</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>297</v>
       </c>
       <c r="C89" t="s">
-        <v>283</v>
+        <v>392</v>
       </c>
       <c r="D89" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>158</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>385</v>
-      </c>
-      <c r="C90" t="s">
-        <v>284</v>
+        <v>153</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>393</v>
       </c>
       <c r="D90" t="s">
-        <v>209</v>
+        <v>154</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>159</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>323</v>
+        <v>155</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>299</v>
       </c>
       <c r="C91" t="s">
-        <v>285</v>
+        <v>394</v>
       </c>
       <c r="D91" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>161</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C92" t="s">
+        <v>157</v>
       </c>
       <c r="D92" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>9</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C93" t="s">
-        <v>214</v>
+        <v>158</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>395</v>
       </c>
       <c r="D93" t="s">
-        <v>10</v>
+        <v>209</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>162</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>331</v>
+        <v>159</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="C94" t="s">
-        <v>220</v>
+        <v>396</v>
       </c>
       <c r="D94" t="s">
-        <v>22</v>
+        <v>160</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>163</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="C95" t="s">
-        <v>286</v>
+        <v>161</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="D95" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>165</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>324</v>
+        <v>9</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C96" t="s">
-        <v>287</v>
+        <v>335</v>
       </c>
       <c r="D96" t="s">
-        <v>166</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>167</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>387</v>
+        <v>162</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="C97" t="s">
-        <v>288</v>
+        <v>341</v>
       </c>
       <c r="D97" t="s">
-        <v>168</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>169</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>388</v>
+        <v>163</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>210</v>
       </c>
       <c r="C98" t="s">
-        <v>270</v>
+        <v>220</v>
       </c>
       <c r="D98" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>171</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>389</v>
-      </c>
-      <c r="C99" t="s">
-        <v>289</v>
+        <v>165</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>397</v>
       </c>
       <c r="D99" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>173</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="C100" t="s">
-        <v>290</v>
+        <v>167</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>398</v>
       </c>
       <c r="D100" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>175</v>
-      </c>
-      <c r="B101" s="4" t="s">
-        <v>391</v>
+        <v>169</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>304</v>
       </c>
       <c r="C101" t="s">
-        <v>291</v>
+        <v>169</v>
       </c>
       <c r="D101" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>177</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="C102" t="s">
-        <v>292</v>
+        <v>171</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>399</v>
       </c>
       <c r="D102" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>179</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>392</v>
+        <v>173</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>306</v>
       </c>
       <c r="C103" t="s">
-        <v>293</v>
+        <v>400</v>
       </c>
       <c r="D103" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>181</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>326</v>
+        <v>175</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>307</v>
       </c>
       <c r="C104" t="s">
-        <v>294</v>
+        <v>401</v>
       </c>
       <c r="D104" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>183</v>
-      </c>
-      <c r="B105" s="4" t="s">
-        <v>393</v>
+        <v>177</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>241</v>
       </c>
       <c r="C105" t="s">
-        <v>295</v>
+        <v>402</v>
       </c>
       <c r="D105" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>185</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>394</v>
+        <v>179</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>308</v>
       </c>
       <c r="C106" t="s">
-        <v>296</v>
+        <v>403</v>
       </c>
       <c r="D106" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>187</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="C107" t="s">
-        <v>188</v>
+        <v>181</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>404</v>
       </c>
       <c r="D107" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>189</v>
-      </c>
-      <c r="B108" s="4" t="s">
-        <v>396</v>
+        <v>183</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>309</v>
       </c>
       <c r="C108" t="s">
-        <v>297</v>
+        <v>405</v>
       </c>
       <c r="D108" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>196</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>397</v>
+        <v>185</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>310</v>
       </c>
       <c r="C109" t="s">
-        <v>298</v>
+        <v>406</v>
       </c>
       <c r="D109" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>191</v>
-      </c>
-      <c r="B110" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="C110" t="s">
-        <v>299</v>
+        <v>187</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>407</v>
       </c>
       <c r="D110" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>198</v>
-      </c>
-      <c r="B111" s="4" t="s">
-        <v>399</v>
-      </c>
-      <c r="C111" t="s">
-        <v>300</v>
+        <v>189</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>408</v>
       </c>
       <c r="D111" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>192</v>
-      </c>
-      <c r="B112" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="C112" t="s">
-        <v>301</v>
+        <v>196</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C112" s="9" t="s">
+        <v>409</v>
       </c>
       <c r="D112" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>194</v>
-      </c>
-      <c r="B113" s="4" t="s">
-        <v>401</v>
+        <v>191</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>314</v>
       </c>
       <c r="C113" t="s">
-        <v>302</v>
+        <v>410</v>
       </c>
       <c r="D113" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>200</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>327</v>
+        <v>198</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>315</v>
       </c>
       <c r="C114" t="s">
-        <v>303</v>
+        <v>221</v>
       </c>
       <c r="D114" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>202</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="C115" t="s">
-        <v>304</v>
+        <v>192</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C115" s="9" t="s">
+        <v>411</v>
       </c>
       <c r="D115" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>194</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C116" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="D116" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>200</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C117" t="s">
+        <v>413</v>
+      </c>
+      <c r="D117" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>202</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C118" t="s">
+        <v>414</v>
+      </c>
+      <c r="D118" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>204</v>
       </c>
-      <c r="B116" s="4" t="s">
-        <v>403</v>
-      </c>
-      <c r="C116" t="s">
-        <v>305</v>
-      </c>
-      <c r="D116" t="s">
+      <c r="B119" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="C119" t="s">
+        <v>415</v>
+      </c>
+      <c r="D119" t="s">
         <v>205</v>
       </c>
     </row>
@@ -3229,7 +3312,7 @@
   <mergeCells count="3">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
completed translations for now
</commit_message>
<xml_diff>
--- a/localisation/App_Localization.xlsx
+++ b/localisation/App_Localization.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="11480" yWindow="0" windowWidth="25600" windowHeight="22040"/>
+    <workbookView xWindow="11475" yWindow="0" windowWidth="25605" windowHeight="18240"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="754">
   <si>
     <t>Meeting App</t>
   </si>
@@ -2226,9 +2226,6 @@
     <t>Espagnol, Allemand...</t>
   </si>
   <si>
-    <t>Spaans, Duits...</t>
-  </si>
-  <si>
     <t>Spanisch, Deutsch, Irisch...</t>
   </si>
   <si>
@@ -2236,6 +2233,54 @@
   </si>
   <si>
     <t>Spanish, German, Irish...</t>
+  </si>
+  <si>
+    <t>Identification d'utilisateur actuel</t>
+  </si>
+  <si>
+    <t>Mod. Rankin Schaal</t>
+  </si>
+  <si>
+    <t>Nieuw contact</t>
+  </si>
+  <si>
+    <t>Nouveau contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bursectomie </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contactbeeld </t>
+  </si>
+  <si>
+    <t xml:space="preserve">% is nu in uw contacten lijst </t>
+  </si>
+  <si>
+    <t>Spaans, Duits, Iers...</t>
+  </si>
+  <si>
+    <t>% van de informatie is nu opgeslagen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK, % is geen contact meer </t>
+  </si>
+  <si>
+    <t>Toegangsrechten voor % zijn opgeslagen</t>
+  </si>
+  <si>
+    <t>% a été ajouté à votre liste de contact</t>
+  </si>
+  <si>
+    <t>Les informations concernant % ont bien été sauvegardées</t>
+  </si>
+  <si>
+    <t>OK, % ne fait plus partie de vos contacts</t>
+  </si>
+  <si>
+    <t>Les droits d'accès pour % ont été sauvegardés</t>
+  </si>
+  <si>
+    <t>Image du contact</t>
   </si>
 </sst>
 </file>
@@ -2279,7 +2324,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2295,6 +2340,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2335,7 +2386,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2343,38 +2394,100 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="25">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2684,20 +2797,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E207"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A209" sqref="A209"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2714,16 +2827,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2737,7 +2850,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2751,7 +2864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2765,7 +2878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2779,7 +2892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2793,7 +2906,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2807,7 +2920,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2821,7 +2934,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2835,7 +2948,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2849,7 +2962,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -2863,7 +2976,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2877,7 +2990,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -2891,7 +3004,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -2905,7 +3018,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2919,16 +3032,16 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -2942,7 +3055,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -2956,7 +3069,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -2970,7 +3083,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -2984,7 +3097,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -2998,7 +3111,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -3012,7 +3125,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>311</v>
       </c>
@@ -3026,7 +3139,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>312</v>
       </c>
@@ -3040,7 +3153,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>315</v>
       </c>
@@ -3054,7 +3167,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -3068,7 +3181,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -3082,16 +3195,16 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="5" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>715</v>
       </c>
@@ -3105,7 +3218,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>486</v>
       </c>
@@ -3119,7 +3232,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>522</v>
       </c>
@@ -3133,7 +3246,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>402</v>
       </c>
@@ -3147,7 +3260,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>536</v>
       </c>
@@ -3161,7 +3274,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>149</v>
       </c>
@@ -3175,7 +3288,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>707</v>
       </c>
@@ -3189,7 +3302,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>451</v>
       </c>
@@ -3203,7 +3316,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>508</v>
       </c>
@@ -3217,7 +3330,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>437</v>
       </c>
@@ -3231,7 +3344,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>453</v>
       </c>
@@ -3245,7 +3358,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>424</v>
       </c>
@@ -3259,7 +3372,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>125</v>
       </c>
@@ -3273,7 +3386,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>407</v>
       </c>
@@ -3287,7 +3400,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>420</v>
       </c>
@@ -3301,7 +3414,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>189</v>
       </c>
@@ -3315,7 +3428,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>474</v>
       </c>
@@ -3329,7 +3442,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>472</v>
       </c>
@@ -3343,7 +3456,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>93</v>
       </c>
@@ -3357,7 +3470,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>445</v>
       </c>
@@ -3371,19 +3484,21 @@
         <v>446</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>449</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="C50" s="3"/>
+      <c r="C50" s="5" t="s">
+        <v>742</v>
+      </c>
       <c r="D50" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>156</v>
       </c>
@@ -3397,7 +3512,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>164</v>
       </c>
@@ -3411,7 +3526,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>699</v>
       </c>
@@ -3425,7 +3540,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>422</v>
       </c>
@@ -3439,7 +3554,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>91</v>
       </c>
@@ -3453,7 +3568,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>82</v>
       </c>
@@ -3467,7 +3582,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>500</v>
       </c>
@@ -3481,7 +3596,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>531</v>
       </c>
@@ -3495,7 +3610,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>44</v>
       </c>
@@ -3509,17 +3624,21 @@
         <v>718</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>721</v>
       </c>
-      <c r="B60" s="2"/>
-      <c r="C60" s="3"/>
+      <c r="B60" s="6" t="s">
+        <v>753</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>743</v>
+      </c>
       <c r="D60" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -3533,7 +3652,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>9</v>
       </c>
@@ -3547,7 +3666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>83</v>
       </c>
@@ -3561,7 +3680,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>410</v>
       </c>
@@ -3575,7 +3694,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>518</v>
       </c>
@@ -3589,11 +3708,13 @@
         <v>519</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>506</v>
       </c>
-      <c r="B66" s="2"/>
+      <c r="B66" s="6" t="s">
+        <v>738</v>
+      </c>
       <c r="C66" s="3" t="s">
         <v>627</v>
       </c>
@@ -3601,7 +3722,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>534</v>
       </c>
@@ -3615,7 +3736,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -3629,7 +3750,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>498</v>
       </c>
@@ -3643,7 +3764,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>678</v>
       </c>
@@ -3657,7 +3778,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>682</v>
       </c>
@@ -3671,7 +3792,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>510</v>
       </c>
@@ -3685,7 +3806,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>425</v>
       </c>
@@ -3699,7 +3820,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>462</v>
       </c>
@@ -3713,7 +3834,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>697</v>
       </c>
@@ -3727,7 +3848,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>504</v>
       </c>
@@ -3741,7 +3862,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>166</v>
       </c>
@@ -3755,7 +3876,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>406</v>
       </c>
@@ -3769,7 +3890,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -3783,7 +3904,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>70</v>
       </c>
@@ -3797,7 +3918,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>178</v>
       </c>
@@ -3811,7 +3932,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>502</v>
       </c>
@@ -3825,7 +3946,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>113</v>
       </c>
@@ -3839,7 +3960,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>131</v>
       </c>
@@ -3853,7 +3974,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>130</v>
       </c>
@@ -3867,7 +3988,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>141</v>
       </c>
@@ -3881,7 +4002,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>172</v>
       </c>
@@ -3895,7 +4016,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>63</v>
       </c>
@@ -3909,7 +4030,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>51</v>
       </c>
@@ -3923,7 +4044,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>159</v>
       </c>
@@ -3937,7 +4058,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>2</v>
       </c>
@@ -3951,7 +4072,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>59</v>
       </c>
@@ -3965,7 +4086,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>160</v>
       </c>
@@ -3979,7 +4100,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>4</v>
       </c>
@@ -3993,7 +4114,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>426</v>
       </c>
@@ -4007,7 +4128,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>466</v>
       </c>
@@ -4021,7 +4142,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>180</v>
       </c>
@@ -4035,7 +4156,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>145</v>
       </c>
@@ -4049,7 +4170,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>157</v>
       </c>
@@ -4063,7 +4184,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>480</v>
       </c>
@@ -4077,7 +4198,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>186</v>
       </c>
@@ -4091,7 +4212,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>492</v>
       </c>
@@ -4105,7 +4226,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>457</v>
       </c>
@@ -4119,7 +4240,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>516</v>
       </c>
@@ -4133,7 +4254,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>432</v>
       </c>
@@ -4147,7 +4268,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>468</v>
       </c>
@@ -4161,7 +4282,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>103</v>
       </c>
@@ -4175,7 +4296,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>55</v>
       </c>
@@ -4189,7 +4310,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>143</v>
       </c>
@@ -4203,7 +4324,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>482</v>
       </c>
@@ -4217,7 +4338,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>414</v>
       </c>
@@ -4231,7 +4352,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>538</v>
       </c>
@@ -4245,7 +4366,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>45</v>
       </c>
@@ -4259,7 +4380,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>711</v>
       </c>
@@ -4273,7 +4394,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>11</v>
       </c>
@@ -4287,7 +4408,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>464</v>
       </c>
@@ -4301,7 +4422,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>118</v>
       </c>
@@ -4315,7 +4436,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>61</v>
       </c>
@@ -4329,7 +4450,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>105</v>
       </c>
@@ -4343,7 +4464,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>107</v>
       </c>
@@ -4357,7 +4478,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>127</v>
       </c>
@@ -4371,7 +4492,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>428</v>
       </c>
@@ -4385,7 +4506,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>53</v>
       </c>
@@ -4399,7 +4520,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>435</v>
       </c>
@@ -4413,7 +4534,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>72</v>
       </c>
@@ -4427,7 +4548,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>151</v>
       </c>
@@ -4441,19 +4562,21 @@
         <v>152</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>430</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="C127" s="3"/>
+      <c r="C127" s="5" t="s">
+        <v>739</v>
+      </c>
       <c r="D127" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>89</v>
       </c>
@@ -4467,7 +4590,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>170</v>
       </c>
@@ -4481,7 +4604,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>496</v>
       </c>
@@ -4495,7 +4618,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>99</v>
       </c>
@@ -4509,17 +4632,21 @@
         <v>100</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>719</v>
       </c>
-      <c r="B132" s="2"/>
-      <c r="C132" s="3"/>
+      <c r="B132" s="6" t="s">
+        <v>741</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>740</v>
+      </c>
       <c r="D132" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>520</v>
       </c>
@@ -4533,7 +4660,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>703</v>
       </c>
@@ -4547,7 +4674,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>439</v>
       </c>
@@ -4561,7 +4688,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>78</v>
       </c>
@@ -4575,7 +4702,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>168</v>
       </c>
@@ -4589,7 +4716,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>176</v>
       </c>
@@ -4603,7 +4730,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>494</v>
       </c>
@@ -4617,7 +4744,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>147</v>
       </c>
@@ -4631,7 +4758,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>30</v>
       </c>
@@ -4645,7 +4772,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>49</v>
       </c>
@@ -4659,7 +4786,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>71</v>
       </c>
@@ -4673,7 +4800,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>527</v>
       </c>
@@ -4687,7 +4814,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>458</v>
       </c>
@@ -4701,7 +4828,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>434</v>
       </c>
@@ -4715,7 +4842,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>121</v>
       </c>
@@ -4729,7 +4856,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>85</v>
       </c>
@@ -4743,7 +4870,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>80</v>
       </c>
@@ -4757,7 +4884,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>57</v>
       </c>
@@ -4771,7 +4898,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>115</v>
       </c>
@@ -4785,7 +4912,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>137</v>
       </c>
@@ -4799,7 +4926,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>418</v>
       </c>
@@ -4813,7 +4940,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>470</v>
       </c>
@@ -4827,7 +4954,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>460</v>
       </c>
@@ -4841,7 +4968,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>523</v>
       </c>
@@ -4855,7 +4982,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>162</v>
       </c>
@@ -4869,7 +4996,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>174</v>
       </c>
@@ -4883,7 +5010,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>74</v>
       </c>
@@ -4897,7 +5024,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>184</v>
       </c>
@@ -4911,7 +5038,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>191</v>
       </c>
@@ -4925,7 +5052,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="162" spans="1:4">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>133</v>
       </c>
@@ -4939,7 +5066,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="163" spans="1:4">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>155</v>
       </c>
@@ -4953,7 +5080,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="164" spans="1:4">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>196</v>
       </c>
@@ -4967,7 +5094,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>488</v>
       </c>
@@ -4981,7 +5108,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>443</v>
       </c>
@@ -4995,7 +5122,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>416</v>
       </c>
@@ -5009,7 +5136,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>476</v>
       </c>
@@ -5023,7 +5150,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="169" spans="1:4">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>512</v>
       </c>
@@ -5037,7 +5164,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="170" spans="1:4">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>200</v>
       </c>
@@ -5051,7 +5178,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="171" spans="1:4">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>198</v>
       </c>
@@ -5065,7 +5192,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>109</v>
       </c>
@@ -5079,7 +5206,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="173" spans="1:4">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>484</v>
       </c>
@@ -5093,7 +5220,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="174" spans="1:4">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>514</v>
       </c>
@@ -5107,7 +5234,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="175" spans="1:4">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>412</v>
       </c>
@@ -5121,7 +5248,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>101</v>
       </c>
@@ -5135,7 +5262,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="177" spans="1:4">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>87</v>
       </c>
@@ -5149,7 +5276,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="178" spans="1:4">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>194</v>
       </c>
@@ -5163,7 +5290,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="179" spans="1:4">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>76</v>
       </c>
@@ -5177,7 +5304,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="180" spans="1:4">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>441</v>
       </c>
@@ -5191,7 +5318,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="181" spans="1:4">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>447</v>
       </c>
@@ -5205,7 +5332,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="182" spans="1:4">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>5</v>
       </c>
@@ -5219,7 +5346,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="183" spans="1:4">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>139</v>
       </c>
@@ -5233,7 +5360,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="184" spans="1:4">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>182</v>
       </c>
@@ -5247,7 +5374,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:4">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>123</v>
       </c>
@@ -5261,7 +5388,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="186" spans="1:4">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>686</v>
       </c>
@@ -5275,7 +5402,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="187" spans="1:4">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>690</v>
       </c>
@@ -5289,7 +5416,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="188" spans="1:4">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>693</v>
       </c>
@@ -5303,7 +5430,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="189" spans="1:4">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>134</v>
       </c>
@@ -5317,7 +5444,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="190" spans="1:4">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>119</v>
       </c>
@@ -5331,7 +5458,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="191" spans="1:4">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>69</v>
       </c>
@@ -5345,7 +5472,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="192" spans="1:4">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>408</v>
       </c>
@@ -5359,7 +5486,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="193" spans="1:4">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>455</v>
       </c>
@@ -5373,7 +5500,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="194" spans="1:4">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>529</v>
       </c>
@@ -5387,7 +5514,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="195" spans="1:4">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>478</v>
       </c>
@@ -5401,7 +5528,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="196" spans="1:4">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>188</v>
       </c>
@@ -5415,7 +5542,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="197" spans="1:4">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>490</v>
       </c>
@@ -5429,7 +5556,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="198" spans="1:4">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>153</v>
       </c>
@@ -5443,7 +5570,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="199" spans="1:4">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>111</v>
       </c>
@@ -5457,7 +5584,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="200" spans="1:4">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>525</v>
       </c>
@@ -5471,7 +5598,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="201" spans="1:4">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>47</v>
       </c>
@@ -5485,9 +5612,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="202" spans="1:4">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B202" s="2" t="s">
         <v>732</v>
@@ -5499,47 +5626,71 @@
         <v>731</v>
       </c>
     </row>
-    <row r="203" spans="1:4">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>734</v>
       </c>
       <c r="C203" s="3" t="s">
+        <v>745</v>
+      </c>
+      <c r="D203" t="s">
         <v>735</v>
       </c>
-      <c r="D203" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4">
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>723</v>
       </c>
+      <c r="B204" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="C204" s="5" t="s">
+        <v>744</v>
+      </c>
       <c r="D204" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="205" spans="1:4">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>724</v>
       </c>
+      <c r="B205" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="C205" s="5" t="s">
+        <v>746</v>
+      </c>
       <c r="D205" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="206" spans="1:4">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>725</v>
       </c>
+      <c r="B206" s="5" t="s">
+        <v>751</v>
+      </c>
+      <c r="C206" s="5" t="s">
+        <v>747</v>
+      </c>
       <c r="D206" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="207" spans="1:4">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>726</v>
+      </c>
+      <c r="B207" s="5" t="s">
+        <v>752</v>
+      </c>
+      <c r="C207" s="5" t="s">
+        <v>748</v>
       </c>
       <c r="D207" t="s">
         <v>730</v>
@@ -5551,8 +5702,23 @@
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A29:E29"/>
   </mergeCells>
-  <conditionalFormatting sqref="A30:E207">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="A30:E59 A204:A207 C204:E207 A67:E203 A66 C66:E66 A61:E65 A60 C60:E60">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B204:B207">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B66">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B60">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed %s placeholder in translations
</commit_message>
<xml_diff>
--- a/localisation/App_Localization.xlsx
+++ b/localisation/App_Localization.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11475" yWindow="0" windowWidth="25605" windowHeight="18240"/>
+    <workbookView xWindow="11480" yWindow="0" windowWidth="25600" windowHeight="18240"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2253,41 +2253,41 @@
     <t xml:space="preserve">Contactbeeld </t>
   </si>
   <si>
-    <t xml:space="preserve">% is nu in uw contacten lijst </t>
-  </si>
-  <si>
     <t>Spaans, Duits, Iers...</t>
   </si>
   <si>
-    <t>% van de informatie is nu opgeslagen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OK, % is geen contact meer </t>
-  </si>
-  <si>
-    <t>Toegangsrechten voor % zijn opgeslagen</t>
-  </si>
-  <si>
-    <t>% a été ajouté à votre liste de contact</t>
-  </si>
-  <si>
-    <t>Les informations concernant % ont bien été sauvegardées</t>
-  </si>
-  <si>
-    <t>OK, % ne fait plus partie de vos contacts</t>
-  </si>
-  <si>
-    <t>Les droits d'accès pour % ont été sauvegardés</t>
-  </si>
-  <si>
     <t>Image du contact</t>
+  </si>
+  <si>
+    <t>%s a été ajouté à votre liste de contact</t>
+  </si>
+  <si>
+    <t>Les informations concernant %s ont bien été sauvegardées</t>
+  </si>
+  <si>
+    <t>OK, %s ne fait plus partie de vos contacts</t>
+  </si>
+  <si>
+    <t>Les droits d'accès pour %s ont été sauvegardés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%s is nu in uw contacten lijst </t>
+  </si>
+  <si>
+    <t>%s van de informatie is nu opgeslagen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK, %s is geen contact meer </t>
+  </si>
+  <si>
+    <t>Toegangsrechten voor %s zijn opgeslagen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2323,8 +2323,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2343,12 +2350,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2359,8 +2360,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2394,70 +2397,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="25">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+  <cellStyles count="27">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2797,20 +2772,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E207"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A209" sqref="A209"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2827,16 +2802,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2850,7 +2825,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2864,7 +2839,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2878,7 +2853,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2892,7 +2867,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2906,7 +2881,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2920,7 +2895,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2934,7 +2909,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2948,7 +2923,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2962,7 +2937,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -2976,7 +2951,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2990,7 +2965,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -3004,7 +2979,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -3018,7 +2993,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -3032,16 +3007,16 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -3055,7 +3030,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -3069,7 +3044,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -3083,7 +3058,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -3097,7 +3072,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -3111,7 +3086,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -3125,7 +3100,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>311</v>
       </c>
@@ -3139,7 +3114,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>312</v>
       </c>
@@ -3153,7 +3128,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>315</v>
       </c>
@@ -3167,7 +3142,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -3181,7 +3156,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -3195,16 +3170,16 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+    <row r="29" spans="1:5">
+      <c r="A29" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>715</v>
       </c>
@@ -3218,7 +3193,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>486</v>
       </c>
@@ -3232,7 +3207,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>522</v>
       </c>
@@ -3246,7 +3221,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>402</v>
       </c>
@@ -3260,7 +3235,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>536</v>
       </c>
@@ -3274,7 +3249,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>149</v>
       </c>
@@ -3288,7 +3263,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>707</v>
       </c>
@@ -3302,7 +3277,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>451</v>
       </c>
@@ -3316,7 +3291,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>508</v>
       </c>
@@ -3330,7 +3305,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>437</v>
       </c>
@@ -3344,7 +3319,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>453</v>
       </c>
@@ -3358,7 +3333,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>424</v>
       </c>
@@ -3372,7 +3347,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>125</v>
       </c>
@@ -3386,7 +3361,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>407</v>
       </c>
@@ -3400,7 +3375,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>420</v>
       </c>
@@ -3414,7 +3389,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>189</v>
       </c>
@@ -3428,7 +3403,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>474</v>
       </c>
@@ -3442,7 +3417,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>472</v>
       </c>
@@ -3456,7 +3431,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>93</v>
       </c>
@@ -3470,7 +3445,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>445</v>
       </c>
@@ -3484,25 +3459,25 @@
         <v>446</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>449</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="6" t="s">
         <v>551</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="3" t="s">
         <v>742</v>
       </c>
       <c r="D50" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>156</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="6" t="s">
         <v>292</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -3512,11 +3487,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>164</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="6" t="s">
         <v>294</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -3526,11 +3501,11 @@
         <v>165</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>699</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="6" t="s">
         <v>700</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -3540,11 +3515,11 @@
         <v>702</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>422</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="6" t="s">
         <v>552</v>
       </c>
       <c r="C54" s="3" t="s">
@@ -3554,11 +3529,11 @@
         <v>423</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>91</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="6" t="s">
         <v>266</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -3568,11 +3543,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>82</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="6" t="s">
         <v>225</v>
       </c>
       <c r="C56" s="3" t="s">
@@ -3582,11 +3557,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>500</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="6" t="s">
         <v>553</v>
       </c>
       <c r="C57" s="3" t="s">
@@ -3596,11 +3571,11 @@
         <v>501</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>531</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="6" t="s">
         <v>554</v>
       </c>
       <c r="C58" s="3" t="s">
@@ -3610,11 +3585,11 @@
         <v>532</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>44</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="6" t="s">
         <v>221</v>
       </c>
       <c r="C59" s="3" t="s">
@@ -3624,25 +3599,25 @@
         <v>718</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>721</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>753</v>
-      </c>
-      <c r="C60" s="5" t="s">
+        <v>745</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>743</v>
       </c>
       <c r="D60" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>67</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="6" t="s">
         <v>223</v>
       </c>
       <c r="C61" s="3" t="s">
@@ -3652,11 +3627,11 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>9</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C62" s="3" t="s">
@@ -3666,11 +3641,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="6" t="s">
         <v>226</v>
       </c>
       <c r="C63" s="3" t="s">
@@ -3680,11 +3655,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>410</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="6" t="s">
         <v>555</v>
       </c>
       <c r="C64" s="3" t="s">
@@ -3694,11 +3669,11 @@
         <v>411</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>518</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="6" t="s">
         <v>556</v>
       </c>
       <c r="C65" s="3" t="s">
@@ -3708,7 +3683,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>506</v>
       </c>
@@ -3722,7 +3697,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>534</v>
       </c>
@@ -3736,7 +3711,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -3750,7 +3725,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>498</v>
       </c>
@@ -3764,7 +3739,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>678</v>
       </c>
@@ -3778,7 +3753,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>682</v>
       </c>
@@ -3792,7 +3767,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>510</v>
       </c>
@@ -3806,7 +3781,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>425</v>
       </c>
@@ -3820,7 +3795,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>462</v>
       </c>
@@ -3834,7 +3809,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>697</v>
       </c>
@@ -3848,7 +3823,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>504</v>
       </c>
@@ -3862,7 +3837,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>166</v>
       </c>
@@ -3876,7 +3851,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>406</v>
       </c>
@@ -3890,7 +3865,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -3904,7 +3879,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>70</v>
       </c>
@@ -3918,7 +3893,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>178</v>
       </c>
@@ -3932,7 +3907,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
         <v>502</v>
       </c>
@@ -3946,7 +3921,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
         <v>113</v>
       </c>
@@ -3960,7 +3935,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
         <v>131</v>
       </c>
@@ -3974,7 +3949,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>130</v>
       </c>
@@ -3988,7 +3963,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
         <v>141</v>
       </c>
@@ -4002,7 +3977,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
         <v>172</v>
       </c>
@@ -4016,7 +3991,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
         <v>63</v>
       </c>
@@ -4030,7 +4005,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
         <v>51</v>
       </c>
@@ -4044,7 +4019,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="15">
       <c r="A90" t="s">
         <v>159</v>
       </c>
@@ -4058,7 +4033,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
         <v>2</v>
       </c>
@@ -4072,7 +4047,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
         <v>59</v>
       </c>
@@ -4086,7 +4061,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
         <v>160</v>
       </c>
@@ -4100,7 +4075,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
         <v>4</v>
       </c>
@@ -4114,7 +4089,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95" t="s">
         <v>426</v>
       </c>
@@ -4128,7 +4103,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
         <v>466</v>
       </c>
@@ -4142,7 +4117,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>180</v>
       </c>
@@ -4156,7 +4131,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>145</v>
       </c>
@@ -4170,7 +4145,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>157</v>
       </c>
@@ -4184,7 +4159,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>480</v>
       </c>
@@ -4198,7 +4173,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>186</v>
       </c>
@@ -4212,7 +4187,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>492</v>
       </c>
@@ -4226,7 +4201,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
         <v>457</v>
       </c>
@@ -4240,7 +4215,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>516</v>
       </c>
@@ -4254,7 +4229,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>432</v>
       </c>
@@ -4268,7 +4243,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
         <v>468</v>
       </c>
@@ -4282,21 +4257,21 @@
         <v>469</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
         <v>103</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C107" s="7" t="s">
         <v>361</v>
       </c>
       <c r="D107" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
         <v>55</v>
       </c>
@@ -4310,7 +4285,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
         <v>143</v>
       </c>
@@ -4324,7 +4299,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
         <v>482</v>
       </c>
@@ -4338,7 +4313,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
         <v>414</v>
       </c>
@@ -4352,7 +4327,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
         <v>538</v>
       </c>
@@ -4366,7 +4341,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
         <v>45</v>
       </c>
@@ -4380,7 +4355,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
         <v>711</v>
       </c>
@@ -4394,7 +4369,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
         <v>11</v>
       </c>
@@ -4408,7 +4383,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
         <v>464</v>
       </c>
@@ -4422,7 +4397,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
         <v>118</v>
       </c>
@@ -4436,7 +4411,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4">
       <c r="A118" t="s">
         <v>61</v>
       </c>
@@ -4450,7 +4425,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4">
       <c r="A119" t="s">
         <v>105</v>
       </c>
@@ -4464,7 +4439,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4">
       <c r="A120" t="s">
         <v>107</v>
       </c>
@@ -4478,7 +4453,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4">
       <c r="A121" t="s">
         <v>127</v>
       </c>
@@ -4492,7 +4467,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4">
       <c r="A122" t="s">
         <v>428</v>
       </c>
@@ -4506,7 +4481,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4">
       <c r="A123" t="s">
         <v>53</v>
       </c>
@@ -4520,7 +4495,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4">
       <c r="A124" t="s">
         <v>435</v>
       </c>
@@ -4534,7 +4509,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4">
       <c r="A125" t="s">
         <v>72</v>
       </c>
@@ -4548,7 +4523,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
         <v>151</v>
       </c>
@@ -4562,25 +4537,25 @@
         <v>152</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4">
       <c r="A127" t="s">
         <v>430</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B127" s="6" t="s">
         <v>582</v>
       </c>
-      <c r="C127" s="5" t="s">
+      <c r="C127" s="3" t="s">
         <v>739</v>
       </c>
       <c r="D127" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4">
       <c r="A128" t="s">
         <v>89</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B128" s="6" t="s">
         <v>265</v>
       </c>
       <c r="C128" s="3" t="s">
@@ -4590,11 +4565,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4">
       <c r="A129" t="s">
         <v>170</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="B129" s="6" t="s">
         <v>297</v>
       </c>
       <c r="C129" s="3" t="s">
@@ -4604,11 +4579,11 @@
         <v>171</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4">
       <c r="A130" t="s">
         <v>496</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="B130" s="6" t="s">
         <v>583</v>
       </c>
       <c r="C130" s="3" t="s">
@@ -4618,11 +4593,11 @@
         <v>497</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4">
       <c r="A131" t="s">
         <v>99</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B131" s="6" t="s">
         <v>266</v>
       </c>
       <c r="C131" s="3" t="s">
@@ -4632,21 +4607,21 @@
         <v>100</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4">
       <c r="A132" t="s">
         <v>719</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>741</v>
       </c>
-      <c r="C132" s="5" t="s">
+      <c r="C132" s="3" t="s">
         <v>740</v>
       </c>
       <c r="D132" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4">
       <c r="A133" t="s">
         <v>520</v>
       </c>
@@ -4660,7 +4635,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4">
       <c r="A134" t="s">
         <v>703</v>
       </c>
@@ -4674,7 +4649,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4">
       <c r="A135" t="s">
         <v>439</v>
       </c>
@@ -4688,7 +4663,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4">
       <c r="A136" t="s">
         <v>78</v>
       </c>
@@ -4702,7 +4677,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4">
       <c r="A137" t="s">
         <v>168</v>
       </c>
@@ -4716,7 +4691,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4">
       <c r="A138" t="s">
         <v>176</v>
       </c>
@@ -4730,7 +4705,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4">
       <c r="A139" t="s">
         <v>494</v>
       </c>
@@ -4744,7 +4719,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4">
       <c r="A140" t="s">
         <v>147</v>
       </c>
@@ -4758,7 +4733,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4">
       <c r="A141" t="s">
         <v>30</v>
       </c>
@@ -4772,7 +4747,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4">
       <c r="A142" t="s">
         <v>49</v>
       </c>
@@ -4786,7 +4761,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4">
       <c r="A143" t="s">
         <v>71</v>
       </c>
@@ -4800,7 +4775,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4">
       <c r="A144" t="s">
         <v>527</v>
       </c>
@@ -4814,7 +4789,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4">
       <c r="A145" t="s">
         <v>458</v>
       </c>
@@ -4828,7 +4803,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4">
       <c r="A146" t="s">
         <v>434</v>
       </c>
@@ -4842,7 +4817,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4">
       <c r="A147" t="s">
         <v>121</v>
       </c>
@@ -4856,7 +4831,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4">
       <c r="A148" t="s">
         <v>85</v>
       </c>
@@ -4870,7 +4845,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4">
       <c r="A149" t="s">
         <v>80</v>
       </c>
@@ -4884,7 +4859,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4">
       <c r="A150" t="s">
         <v>57</v>
       </c>
@@ -4898,7 +4873,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4">
       <c r="A151" t="s">
         <v>115</v>
       </c>
@@ -4912,7 +4887,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4">
       <c r="A152" t="s">
         <v>137</v>
       </c>
@@ -4926,7 +4901,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4">
       <c r="A153" t="s">
         <v>418</v>
       </c>
@@ -4940,7 +4915,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4">
       <c r="A154" t="s">
         <v>470</v>
       </c>
@@ -4954,7 +4929,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4">
       <c r="A155" t="s">
         <v>460</v>
       </c>
@@ -4968,7 +4943,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4">
       <c r="A156" t="s">
         <v>523</v>
       </c>
@@ -4982,7 +4957,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4">
       <c r="A157" t="s">
         <v>162</v>
       </c>
@@ -4996,7 +4971,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4">
       <c r="A158" t="s">
         <v>174</v>
       </c>
@@ -5010,7 +4985,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4">
       <c r="A159" t="s">
         <v>74</v>
       </c>
@@ -5024,7 +4999,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4">
       <c r="A160" t="s">
         <v>184</v>
       </c>
@@ -5038,7 +5013,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4">
       <c r="A161" t="s">
         <v>191</v>
       </c>
@@ -5052,7 +5027,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4">
       <c r="A162" t="s">
         <v>133</v>
       </c>
@@ -5066,7 +5041,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4">
       <c r="A163" t="s">
         <v>155</v>
       </c>
@@ -5080,7 +5055,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4">
       <c r="A164" t="s">
         <v>196</v>
       </c>
@@ -5094,7 +5069,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4">
       <c r="A165" t="s">
         <v>488</v>
       </c>
@@ -5108,7 +5083,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4">
       <c r="A166" t="s">
         <v>443</v>
       </c>
@@ -5122,7 +5097,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4">
       <c r="A167" t="s">
         <v>416</v>
       </c>
@@ -5136,7 +5111,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4">
       <c r="A168" t="s">
         <v>476</v>
       </c>
@@ -5150,7 +5125,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4">
       <c r="A169" t="s">
         <v>512</v>
       </c>
@@ -5164,7 +5139,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4">
       <c r="A170" t="s">
         <v>200</v>
       </c>
@@ -5178,7 +5153,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4">
       <c r="A171" t="s">
         <v>198</v>
       </c>
@@ -5192,7 +5167,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4">
       <c r="A172" t="s">
         <v>109</v>
       </c>
@@ -5206,7 +5181,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4">
       <c r="A173" t="s">
         <v>484</v>
       </c>
@@ -5220,7 +5195,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4">
       <c r="A174" t="s">
         <v>514</v>
       </c>
@@ -5234,7 +5209,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4">
       <c r="A175" t="s">
         <v>412</v>
       </c>
@@ -5248,7 +5223,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4">
       <c r="A176" t="s">
         <v>101</v>
       </c>
@@ -5262,7 +5237,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4">
       <c r="A177" t="s">
         <v>87</v>
       </c>
@@ -5276,7 +5251,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4">
       <c r="A178" t="s">
         <v>194</v>
       </c>
@@ -5290,7 +5265,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4">
       <c r="A179" t="s">
         <v>76</v>
       </c>
@@ -5304,7 +5279,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4">
       <c r="A180" t="s">
         <v>441</v>
       </c>
@@ -5318,7 +5293,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4">
       <c r="A181" t="s">
         <v>447</v>
       </c>
@@ -5332,7 +5307,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4">
       <c r="A182" t="s">
         <v>5</v>
       </c>
@@ -5346,7 +5321,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4">
       <c r="A183" t="s">
         <v>139</v>
       </c>
@@ -5360,7 +5335,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4">
       <c r="A184" t="s">
         <v>182</v>
       </c>
@@ -5374,7 +5349,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4">
       <c r="A185" t="s">
         <v>123</v>
       </c>
@@ -5388,7 +5363,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4">
       <c r="A186" t="s">
         <v>686</v>
       </c>
@@ -5402,7 +5377,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4">
       <c r="A187" t="s">
         <v>690</v>
       </c>
@@ -5416,7 +5391,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4">
       <c r="A188" t="s">
         <v>693</v>
       </c>
@@ -5430,7 +5405,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4">
       <c r="A189" t="s">
         <v>134</v>
       </c>
@@ -5444,7 +5419,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4">
       <c r="A190" t="s">
         <v>119</v>
       </c>
@@ -5458,7 +5433,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4">
       <c r="A191" t="s">
         <v>69</v>
       </c>
@@ -5472,7 +5447,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4">
       <c r="A192" t="s">
         <v>408</v>
       </c>
@@ -5486,7 +5461,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4">
       <c r="A193" t="s">
         <v>455</v>
       </c>
@@ -5500,7 +5475,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4">
       <c r="A194" t="s">
         <v>529</v>
       </c>
@@ -5514,7 +5489,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4">
       <c r="A195" t="s">
         <v>478</v>
       </c>
@@ -5528,7 +5503,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4">
       <c r="A196" t="s">
         <v>188</v>
       </c>
@@ -5542,7 +5517,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4">
       <c r="A197" t="s">
         <v>490</v>
       </c>
@@ -5556,7 +5531,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4">
       <c r="A198" t="s">
         <v>153</v>
       </c>
@@ -5570,7 +5545,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4">
       <c r="A199" t="s">
         <v>111</v>
       </c>
@@ -5584,7 +5559,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4">
       <c r="A200" t="s">
         <v>525</v>
       </c>
@@ -5598,7 +5573,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4">
       <c r="A201" t="s">
         <v>47</v>
       </c>
@@ -5612,7 +5587,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4">
       <c r="A202" t="s">
         <v>736</v>
       </c>
@@ -5626,7 +5601,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4">
       <c r="A203" t="s">
         <v>737</v>
       </c>
@@ -5634,63 +5609,63 @@
         <v>734</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D203" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4">
       <c r="A204" t="s">
         <v>723</v>
       </c>
-      <c r="B204" s="5" t="s">
-        <v>749</v>
-      </c>
-      <c r="C204" s="5" t="s">
-        <v>744</v>
+      <c r="B204" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>750</v>
       </c>
       <c r="D204" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4">
       <c r="A205" t="s">
         <v>724</v>
       </c>
-      <c r="B205" s="5" t="s">
-        <v>750</v>
-      </c>
-      <c r="C205" s="5" t="s">
-        <v>746</v>
+      <c r="B205" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="C205" s="3" t="s">
+        <v>751</v>
       </c>
       <c r="D205" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4">
       <c r="A206" t="s">
         <v>725</v>
       </c>
-      <c r="B206" s="5" t="s">
-        <v>751</v>
-      </c>
-      <c r="C206" s="5" t="s">
-        <v>747</v>
+      <c r="B206" s="3" t="s">
+        <v>748</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>752</v>
       </c>
       <c r="D206" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4">
       <c r="A207" t="s">
         <v>726</v>
       </c>
-      <c r="B207" s="5" t="s">
-        <v>752</v>
-      </c>
-      <c r="C207" s="5" t="s">
-        <v>748</v>
+      <c r="B207" s="3" t="s">
+        <v>749</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>753</v>
       </c>
       <c r="D207" t="s">
         <v>730</v>
@@ -5702,23 +5677,23 @@
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A29:E29"/>
   </mergeCells>
-  <conditionalFormatting sqref="A30:E59 A204:A207 C204:E207 A67:E203 A66 C66:E66 A61:E65 A60 C60:E60">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+  <conditionalFormatting sqref="A30:E59 A204:A207 C204:E207 A67:E106 A66 C66:E66 A61:E65 A60 C60:E60 A108:E203 A107:B107 D107:E107">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B204:B207">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>